<commit_message>
added long captions to sample xlsx to generate NG result.
</commit_message>
<xml_diff>
--- a/sample/CaptionListSample.xlsx
+++ b/sample/CaptionListSample.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Caption</t>
   </si>
@@ -45,6 +45,32 @@
   </si>
   <si>
     <t>目的地</t>
+  </si>
+  <si>
+    <t>-----Destination-----</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">-----</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">目的地</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-----</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -54,7 +80,31 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
+    <font>
+      <sz val="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="128"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -63,22 +113,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="unifont"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -125,12 +160,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,67 +188,90 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.8295454545455"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>